<commit_message>
Short version of plots for Exp 1 and 2
Former-commit-id: a49ebd3737c60895db6e101d16b77790f822d9f9
</commit_message>
<xml_diff>
--- a/Swift_Experiments/strategy_1/analysis/strategy_1_analysis.xlsx
+++ b/Swift_Experiments/strategy_1/analysis/strategy_1_analysis.xlsx
@@ -228,8 +228,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -247,13 +251,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1984,6 +1992,999 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TTCmeasured</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>TTC_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>12520.85245700148</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11133.18142610937</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>17459.32985302319</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>35739.54311403547</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>TTC_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>12520.85245700148</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11133.18142610937</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>17459.32985302319</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>35739.54311403547</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTC_stampede_gordon!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTC_stampede_gordon!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>18496.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13098.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18966.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>TTCideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TTC_stampede_gordon!$M$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4800.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2045912128"/>
+        <c:axId val="-2046738192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2045912128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2046738192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2046738192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2045912128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="2000.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Tw_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>12389.03090102962</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10902.21981601301</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16372.31676489311</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>31494.21464861973</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Tw_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>12389.03090102962</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10902.21981601301</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16372.31676489311</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>31494.21464861973</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tw_stampede_gordon!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tw_stampede_gordon!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16736.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11440.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15777.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60593.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2023951984"/>
+        <c:axId val="1766887072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2023951984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1766887072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1766887072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120000.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2023951984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -2116,6 +3117,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2346,6 +3348,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2472,6 +3475,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2581,7 +3585,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2744,6 +3748,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2971,6 +3976,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3097,6 +4103,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3206,7 +4213,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4068,6 +5075,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -6584,6 +7671,1012 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7179,6 +9272,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>778933</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149013</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8071,10 +10228,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P7"/>
+      <selection activeCell="E13" sqref="E13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8424,8 +10581,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>41107</v>
+      </c>
+      <c r="F13">
+        <v>74328</v>
+      </c>
+      <c r="G13">
+        <v>127092</v>
+      </c>
+      <c r="H13">
+        <v>71073</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8761,8 +10933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A51" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add label with subscripted text to paper diagrams
</commit_message>
<xml_diff>
--- a/Swift_Experiments/strategy_1/analysis/strategy_1_analysis.xlsx
+++ b/Swift_Experiments/strategy_1/analysis/strategy_1_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="17060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="17060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TTC_stampede" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     </textPr>
   </connection>
   <connection id="2" name="Te-Executing_task-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="6" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/Swift_Experiments/strategy_1/analysis/stampede_gordon/Te-Executing_task-stampede_gordon.csv" comma="1">
+    <textPr fileType="mac" firstRow="6" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/Swift_Experiments/strategy_1/analysis/stampede_gordon/Te-Executing_task-stampede_gordon.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -74,7 +74,7 @@
     </textPr>
   </connection>
   <connection id="4" name="TTC-Time_to_completion-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="6" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/Swift_Experiments/strategy_1/analysis/stampede_gordon/TTC-Time_to_completion-stampede_gordon.csv" tab="0" comma="1">
+    <textPr fileType="mac" firstRow="6" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/Swift_Experiments/strategy_1/analysis/stampede_gordon/TTC-Time_to_completion-stampede_gordon.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -94,7 +94,7 @@
     </textPr>
   </connection>
   <connection id="6" name="Tw-Submitting_task-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="6" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/Swift_Experiments/strategy_1/analysis/stampede_gordon/Tw-Submitting_task-stampede_gordon.csv" tab="0" comma="1">
+    <textPr fileType="mac" firstRow="6" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/Swift_Experiments/strategy_1/analysis/stampede_gordon/Tw-Submitting_task-stampede_gordon.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -568,11 +568,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144904624"/>
-        <c:axId val="-2144921680"/>
+        <c:axId val="-1963485648"/>
+        <c:axId val="-2019430304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144904624"/>
+        <c:axId val="-1963485648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144921680"/>
+        <c:crossAx val="-2019430304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -677,7 +677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144921680"/>
+        <c:axId val="-2019430304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000.0"/>
@@ -802,7 +802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144904624"/>
+        <c:crossAx val="-1963485648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2000.0"/>
@@ -1147,11 +1147,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141589552"/>
-        <c:axId val="-2141583520"/>
+        <c:axId val="-2021395872"/>
+        <c:axId val="-2020637200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141589552"/>
+        <c:axId val="-2021395872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,7 +1248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141583520"/>
+        <c:crossAx val="-2020637200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1256,7 +1256,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141583520"/>
+        <c:axId val="-2020637200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000.0"/>
@@ -1382,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141589552"/>
+        <c:crossAx val="-2021395872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1705,11 +1705,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141543648"/>
-        <c:axId val="-2141537744"/>
+        <c:axId val="-1990960080"/>
+        <c:axId val="-1990954192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141543648"/>
+        <c:axId val="-1990960080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1808,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141537744"/>
+        <c:crossAx val="-1990954192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1816,7 +1816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141537744"/>
+        <c:axId val="-1990954192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000.0"/>
@@ -1929,7 +1929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141543648"/>
+        <c:crossAx val="-1990960080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2183,6 +2183,59 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Tw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tw_stampede_gordon!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16736.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11440.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15777.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60593.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2193,11 +2246,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2045912128"/>
-        <c:axId val="-2046738192"/>
+        <c:axId val="-1971186032"/>
+        <c:axId val="-2008981264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2045912128"/>
+        <c:axId val="-1971186032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2294,7 +2347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2046738192"/>
+        <c:crossAx val="-2008981264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2302,7 +2355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2046738192"/>
+        <c:axId val="-2008981264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000.0"/>
@@ -2427,7 +2480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045912128"/>
+        <c:crossAx val="-1971186032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2000.0"/>
@@ -2663,11 +2716,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2023951984"/>
-        <c:axId val="1766887072"/>
+        <c:axId val="-1963263312"/>
+        <c:axId val="-2006517504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2023951984"/>
+        <c:axId val="-1963263312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2764,7 +2817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1766887072"/>
+        <c:crossAx val="-2006517504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2772,7 +2825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1766887072"/>
+        <c:axId val="-2006517504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000.0"/>
@@ -2898,7 +2951,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2023951984"/>
+        <c:crossAx val="-1963263312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3117,7 +3170,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3312,11 +3364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141484176"/>
-        <c:axId val="-2141478272"/>
+        <c:axId val="-2037239888"/>
+        <c:axId val="-1965539456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141484176"/>
+        <c:axId val="-2037239888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3348,7 +3400,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3415,7 +3466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141478272"/>
+        <c:crossAx val="-1965539456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3423,7 +3474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141478272"/>
+        <c:axId val="-1965539456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -3475,7 +3526,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3536,7 +3586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141484176"/>
+        <c:crossAx val="-2037239888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3748,7 +3798,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3940,11 +3989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141441216"/>
-        <c:axId val="-2141435312"/>
+        <c:axId val="-1965811936"/>
+        <c:axId val="-1964137888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141441216"/>
+        <c:axId val="-1965811936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3976,7 +4025,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4043,7 +4091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141435312"/>
+        <c:crossAx val="-1964137888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4051,7 +4099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141435312"/>
+        <c:axId val="-1964137888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -4103,7 +4151,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4164,7 +4211,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141441216"/>
+        <c:crossAx val="-1965811936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4564,11 +4611,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141397392"/>
-        <c:axId val="-2141391488"/>
+        <c:axId val="-1964187488"/>
+        <c:axId val="-1964781920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141397392"/>
+        <c:axId val="-1964187488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4666,7 +4713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141391488"/>
+        <c:crossAx val="-1964781920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4674,7 +4721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141391488"/>
+        <c:axId val="-1964781920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -4786,7 +4833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141397392"/>
+        <c:crossAx val="-1964187488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10230,8 +10277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10933,7 +10980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>

</xml_diff>